<commit_message>
Fix barclaycard format (#22)
</commit_message>
<xml_diff>
--- a/internal/pkg/batchconvert/testfiles/input/mixed/Umsaetze.xlsx
+++ b/internal/pkg/batchconvert/testfiles/input/mixed/Umsaetze.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
   <si>
     <t xml:space="preserve">Transaktionsansicht</t>
   </si>
@@ -109,6 +109,9 @@
     <t xml:space="preserve">Kontaktlose Bezahlung</t>
   </si>
   <si>
+    <t xml:space="preserve">Händlerdetails</t>
+  </si>
+  <si>
     <t xml:space="preserve">98765432109876543210987</t>
   </si>
   <si>
@@ -145,6 +148,9 @@
     <t xml:space="preserve">Visa</t>
   </si>
   <si>
+    <t xml:space="preserve">Händler1</t>
+  </si>
+  <si>
     <t xml:space="preserve">98765432109876543210988</t>
   </si>
   <si>
@@ -160,6 +166,9 @@
     <t xml:space="preserve">XYZ  ROTTERDAM     NL</t>
   </si>
   <si>
+    <t xml:space="preserve">Händler2</t>
+  </si>
+  <si>
     <t xml:space="preserve">98765432109876543210989</t>
   </si>
   <si>
@@ -175,6 +184,9 @@
     <t xml:space="preserve">Abc *Abc def 12345 DE</t>
   </si>
   <si>
+    <t xml:space="preserve">Händler3</t>
+  </si>
+  <si>
     <t xml:space="preserve">98765432109876543210990</t>
   </si>
   <si>
@@ -184,6 +196,9 @@
     <t xml:space="preserve">DB FERNVERKEHR AG      FRANKFURT     DE</t>
   </si>
   <si>
+    <t xml:space="preserve">Händler4</t>
+  </si>
+  <si>
     <t xml:space="preserve">98765432109876543210991</t>
   </si>
   <si>
@@ -199,6 +214,9 @@
     <t xml:space="preserve">Ja</t>
   </si>
   <si>
+    <t xml:space="preserve">Händler5</t>
+  </si>
+  <si>
     <t xml:space="preserve">98765432109876543210992</t>
   </si>
   <si>
@@ -212,6 +230,9 @@
   </si>
   <si>
     <t xml:space="preserve">DB BAHN  A-BC 123ZOO   INTERNET      DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Händler6</t>
   </si>
 </sst>
 </file>
@@ -312,20 +333,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -401,406 +426,537 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:N19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O20" activeCellId="0" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="10.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="13.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="10.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="21.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.63"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="E14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="3" t="s">
+      <c r="H14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L14" s="3" t="s">
+      <c r="I14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="L14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="M14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="I15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="N15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="G16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="3" t="s">
+      <c r="H16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
+      <c r="I16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="L16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="M16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="I17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="D18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="G18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="H18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L16" s="3" t="s">
+      <c r="I18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="L18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="M18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L17" s="3" t="s">
+      <c r="I19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="L19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="N17" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>37</v>
+      <c r="M19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Barclay XLS format
</commit_message>
<xml_diff>
--- a/internal/pkg/batchconvert/testfiles/input/mixed/Umsaetze.xlsx
+++ b/internal/pkg/batchconvert/testfiles/input/mixed/Umsaetze.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
   <si>
     <t xml:space="preserve">Transaktionsansicht</t>
   </si>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Land</t>
   </si>
   <si>
-    <t xml:space="preserve">Name des Karteninhabers</t>
+    <t xml:space="preserve">Karteninhaber</t>
   </si>
   <si>
     <t xml:space="preserve">Kartennetzwerk</t>
@@ -109,7 +109,43 @@
     <t xml:space="preserve">Kontaktlose Bezahlung</t>
   </si>
   <si>
-    <t xml:space="preserve">Händlerdetails</t>
+    <t xml:space="preserve">Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98765432109876543210986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.09.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,75 €</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belastung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vorgemerkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490638******1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5 €</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VORNAME NACHNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detail0</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210987</t>
@@ -118,37 +154,19 @@
     <t xml:space="preserve">28.09.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">29.09.2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">-64,14 €</t>
   </si>
   <si>
     <t xml:space="preserve">PAYPAL *DEALER    98765432   DE</t>
   </si>
   <si>
-    <t xml:space="preserve">Belastung</t>
-  </si>
-  <si>
     <t xml:space="preserve">Berechnet</t>
   </si>
   <si>
-    <t xml:space="preserve">490638******1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nein</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE</t>
   </si>
   <si>
-    <t xml:space="preserve">VORNAME NACHNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Händler1</t>
+    <t xml:space="preserve">Detail1</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210988</t>
@@ -166,7 +184,7 @@
     <t xml:space="preserve">XYZ  ROTTERDAM     NL</t>
   </si>
   <si>
-    <t xml:space="preserve">Händler2</t>
+    <t xml:space="preserve">Detail2</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210989</t>
@@ -184,7 +202,7 @@
     <t xml:space="preserve">Abc *Abc def 12345 DE</t>
   </si>
   <si>
-    <t xml:space="preserve">Händler3</t>
+    <t xml:space="preserve">Detail3</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210990</t>
@@ -196,7 +214,7 @@
     <t xml:space="preserve">DB FERNVERKEHR AG      FRANKFURT     DE</t>
   </si>
   <si>
-    <t xml:space="preserve">Händler4</t>
+    <t xml:space="preserve">Detail4</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210991</t>
@@ -214,7 +232,7 @@
     <t xml:space="preserve">Ja</t>
   </si>
   <si>
-    <t xml:space="preserve">Händler5</t>
+    <t xml:space="preserve">Detail5</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210992</t>
@@ -232,7 +250,7 @@
     <t xml:space="preserve">DB BAHN  A-BC 123ZOO   INTERNET      DE</t>
   </si>
   <si>
-    <t xml:space="preserve">Händler6</t>
+    <t xml:space="preserve">Detail6</t>
   </si>
 </sst>
 </file>
@@ -537,16 +555,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O20" activeCellId="0" sqref="O20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="13.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="10.09"/>
@@ -557,7 +575,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="21.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -679,90 +697,86 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="J14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="N14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="F15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="H15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K15" s="4"/>
       <c r="L15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>38</v>
@@ -788,13 +802,13 @@
         <v>53</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>52</v>
@@ -802,14 +816,12 @@
       <c r="J16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="M16" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>38</v>
@@ -823,87 +835,87 @@
         <v>55</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="I17" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>38</v>
       </c>
       <c r="K17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="M17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M17" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="N17" s="4" t="s">
         <v>38</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="J18" s="4" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="K18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="M18" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>38</v>
@@ -920,43 +932,90 @@
         <v>66</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="K19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="M19" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Barclay XLS format (#91)
</commit_message>
<xml_diff>
--- a/internal/pkg/batchconvert/testfiles/input/mixed/Umsaetze.xlsx
+++ b/internal/pkg/batchconvert/testfiles/input/mixed/Umsaetze.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
   <si>
     <t xml:space="preserve">Transaktionsansicht</t>
   </si>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Land</t>
   </si>
   <si>
-    <t xml:space="preserve">Name des Karteninhabers</t>
+    <t xml:space="preserve">Karteninhaber</t>
   </si>
   <si>
     <t xml:space="preserve">Kartennetzwerk</t>
@@ -109,7 +109,43 @@
     <t xml:space="preserve">Kontaktlose Bezahlung</t>
   </si>
   <si>
-    <t xml:space="preserve">Händlerdetails</t>
+    <t xml:space="preserve">Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98765432109876543210986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.09.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,75 €</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belastung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vorgemerkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490638******1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5 €</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VORNAME NACHNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detail0</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210987</t>
@@ -118,37 +154,19 @@
     <t xml:space="preserve">28.09.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">29.09.2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">-64,14 €</t>
   </si>
   <si>
     <t xml:space="preserve">PAYPAL *DEALER    98765432   DE</t>
   </si>
   <si>
-    <t xml:space="preserve">Belastung</t>
-  </si>
-  <si>
     <t xml:space="preserve">Berechnet</t>
   </si>
   <si>
-    <t xml:space="preserve">490638******1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nein</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE</t>
   </si>
   <si>
-    <t xml:space="preserve">VORNAME NACHNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Händler1</t>
+    <t xml:space="preserve">Detail1</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210988</t>
@@ -166,7 +184,7 @@
     <t xml:space="preserve">XYZ  ROTTERDAM     NL</t>
   </si>
   <si>
-    <t xml:space="preserve">Händler2</t>
+    <t xml:space="preserve">Detail2</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210989</t>
@@ -184,7 +202,7 @@
     <t xml:space="preserve">Abc *Abc def 12345 DE</t>
   </si>
   <si>
-    <t xml:space="preserve">Händler3</t>
+    <t xml:space="preserve">Detail3</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210990</t>
@@ -196,7 +214,7 @@
     <t xml:space="preserve">DB FERNVERKEHR AG      FRANKFURT     DE</t>
   </si>
   <si>
-    <t xml:space="preserve">Händler4</t>
+    <t xml:space="preserve">Detail4</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210991</t>
@@ -214,7 +232,7 @@
     <t xml:space="preserve">Ja</t>
   </si>
   <si>
-    <t xml:space="preserve">Händler5</t>
+    <t xml:space="preserve">Detail5</t>
   </si>
   <si>
     <t xml:space="preserve">98765432109876543210992</t>
@@ -232,7 +250,7 @@
     <t xml:space="preserve">DB BAHN  A-BC 123ZOO   INTERNET      DE</t>
   </si>
   <si>
-    <t xml:space="preserve">Händler6</t>
+    <t xml:space="preserve">Detail6</t>
   </si>
 </sst>
 </file>
@@ -537,16 +555,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O20" activeCellId="0" sqref="O20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="13.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="10.09"/>
@@ -557,7 +575,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="21.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -679,90 +697,86 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="J14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="N14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="F15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="H15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K15" s="4"/>
       <c r="L15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>38</v>
@@ -788,13 +802,13 @@
         <v>53</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>52</v>
@@ -802,14 +816,12 @@
       <c r="J16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="M16" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>38</v>
@@ -823,87 +835,87 @@
         <v>55</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="I17" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>38</v>
       </c>
       <c r="K17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="M17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M17" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="N17" s="4" t="s">
         <v>38</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="J18" s="4" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="K18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="M18" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>38</v>
@@ -920,43 +932,90 @@
         <v>66</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="K19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="M19" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>